<commit_message>
Added NO_FISH to 2016 Calf Island fish data transect 1
</commit_message>
<xml_diff>
--- a/raw_data/KEEN ONE/Byrnes/2016/Calf Island 2016/CalfIsland_fish_2016.xlsx
+++ b/raw_data/KEEN ONE/Byrnes/2016/Calf Island 2016/CalfIsland_fish_2016.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="30660" yWindow="-8000" windowWidth="25520" windowHeight="15600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Data Entry" sheetId="1" r:id="rId1"/>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="144">
   <si>
     <t>YEAR</t>
   </si>
@@ -623,6 +623,9 @@
   </si>
   <si>
     <t>LYMAN</t>
+  </si>
+  <si>
+    <t>NO_FISH</t>
   </si>
 </sst>
 </file>
@@ -719,8 +722,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -828,7 +833,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -852,6 +857,7 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -875,6 +881,7 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1208,7 +1215,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M18" sqref="M18"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1318,7 +1325,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>143</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>

</xml_diff>